<commit_message>
Initial POM framework setup
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/Excel.xlsx
+++ b/src/test/resources/Excel/Excel.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\eclipse-workspace\DataDrivenFramework\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\eclipse-workspace\m4c-testing\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9677A0-7BBF-4CC2-9EE4-1EA8982710EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{349D8BA8-8E5F-4D5D-980A-85297792854E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5100" yWindow="1308" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2700" windowWidth="17280" windowHeight="8964" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MatpatraWebLoginTest" sheetId="1" r:id="rId1"/>
     <sheet name="MatpatraAdminLoginTest" sheetId="4" r:id="rId2"/>
     <sheet name="MatpatraAdminViaOTPTest" sheetId="5" r:id="rId3"/>
-    <sheet name="MatpatraLoginViaEmailTest" sheetId="6" r:id="rId4"/>
+    <sheet name="WebSignInData" sheetId="6" r:id="rId4"/>
     <sheet name="AddCustomer" sheetId="2" r:id="rId5"/>
     <sheet name="OpenAccountTest" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -72,23 +72,38 @@
     <t>IsDuplicate</t>
   </si>
   <si>
-    <t>tatawatvikas7@gmail.com</t>
-  </si>
-  <si>
     <t>Vikas@133</t>
   </si>
   <si>
-    <t>kanta@yopmail.com</t>
-  </si>
-  <si>
-    <t>ptcy888@gmail.com</t>
+    <t>expectedMessage</t>
+  </si>
+  <si>
+    <t>Vikas@122</t>
+  </si>
+  <si>
+    <t>User Name or Mobile is required</t>
+  </si>
+  <si>
+    <t>Login Successfully</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>User Name or Mobile is required|Password is required</t>
+  </si>
+  <si>
+    <t>Invalid registered mobile number or userName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -106,6 +121,20 @@
       <color rgb="FF22191B"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF22191B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,13 +157,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,56 +556,72 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CC6E30-A2A4-46F5-9264-71E9D59BBDAF}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.21875" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>7027440090</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="C3" s="5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="C4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>7027440090</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
+      <c r="C5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>